<commit_message>
Updated Provider_Template and populateProviders
</commit_message>
<xml_diff>
--- a/Provider_Template.xlsx
+++ b/Provider_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Google Drive\UNM\2021_spring\ECE435\project\DD_Branch\ece435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6603F0D5-8B33-4288-83F2-07B4C8538C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF136022-7C5F-4BE5-B4E3-74C0AE8D6506}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>First</t>
   </si>
   <si>
-    <t>CHF</t>
-  </si>
-  <si>
     <t>THS</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   <si>
     <t>MON
 AM</t>
+  </si>
+  <si>
+    <t>CHCF</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:V1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -524,61 +524,61 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="T1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -586,13 +586,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>1</v>
       </c>
       <c r="K2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="3">
         <v>0</v>
@@ -655,13 +655,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
@@ -670,10 +670,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7">
         <v>0</v>
@@ -700,10 +700,10 @@
         <v>0</v>
       </c>
       <c r="Q3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S3" s="7">
         <v>2</v>
@@ -723,19 +723,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -744,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -753,19 +753,19 @@
         <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="3">
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O4" s="3">
         <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="3">
         <v>0</v>
@@ -1773,9 +1773,9 @@
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0"/>
   <dataValidations count="1">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="E2:R1048576" xr:uid="{EB651279-06EB-459E-895C-F6054F350973}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:R1048576" xr:uid="{456F7F48-20F7-4E73-8A50-6134AAE9277C}">
       <formula1>0</formula1>
-      <formula2>2</formula2>
+      <formula2>1</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -1812,49 +1812,49 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Provider dummy data and poopulateProviders
</commit_message>
<xml_diff>
--- a/Provider_Template.xlsx
+++ b/Provider_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Google Drive\UNM\2021_spring\ECE435\project\DD_Branch\ece435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B97283-B02A-473E-8BF2-F519B8987758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BF3DE9-0E27-4585-ABFC-04FE072F0F5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="2475" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
-  <si>
-    <t>Employee ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="56">
   <si>
     <t>Last</t>
   </si>
@@ -49,28 +46,13 @@
     <t>THS</t>
   </si>
   <si>
-    <t>PPHC</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
     <t>Specialties</t>
   </si>
   <si>
-    <t>Ped</t>
-  </si>
-  <si>
     <t>NP</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Adult</t>
   </si>
   <si>
     <t>Specialty</t>
@@ -131,15 +113,6 @@
     <t>Hour Limit</t>
   </si>
   <si>
-    <t>Winning</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>Jane</t>
   </si>
   <si>
@@ -169,13 +142,88 @@
   </si>
   <si>
     <t>SDO</t>
+  </si>
+  <si>
+    <t>Colgan</t>
+  </si>
+  <si>
+    <t>PED</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Zelleke</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Brendan</t>
+  </si>
+  <si>
+    <t>Garza</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Haley</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Veal</t>
+  </si>
+  <si>
+    <t>Chop</t>
+  </si>
+  <si>
+    <t>Wilkerson</t>
+  </si>
+  <si>
+    <t>Stacy</t>
+  </si>
+  <si>
+    <t>Littlejohn</t>
+  </si>
+  <si>
+    <t>Naomi</t>
+  </si>
+  <si>
+    <t>Willie</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Stochosky</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Marsha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,12 +238,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -242,23 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -273,13 +303,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -498,230 +522,834 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1000"/>
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10" style="5" customWidth="1"/>
-    <col min="5" max="18" width="4.625" style="5" customWidth="1"/>
-    <col min="19" max="20" width="7.625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="8.125" style="5" customWidth="1"/>
-    <col min="22" max="29" width="7.625" style="5" customWidth="1"/>
-    <col min="30" max="16384" width="12.625" style="5"/>
+    <col min="1" max="1" width="9.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="4" max="17" width="4.625" style="3" customWidth="1"/>
+    <col min="18" max="25" width="7.625" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="12.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:18" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R12" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f>COLUMN(A25)-1</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" ref="B24:R24" si="0">COLUMN(B25)-1</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="N24" s="3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="O24" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="P24" s="3">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="Q24" s="3">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="R24" s="3">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="6">
-        <v>1</v>
-      </c>
-      <c r="T2" s="6">
-        <v>1</v>
-      </c>
-      <c r="U2" s="6">
-        <v>2</v>
-      </c>
-      <c r="V2" s="5">
-        <f>COLUMN(V1)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>5</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7">
-        <v>2</v>
-      </c>
-      <c r="T3" s="7">
-        <v>0</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0</v>
-      </c>
-      <c r="V3" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="6">
-        <v>1</v>
-      </c>
-      <c r="T4" s="6">
-        <v>1</v>
-      </c>
-      <c r="U4" s="6">
-        <v>2</v>
-      </c>
-      <c r="V4" s="5">
-        <f>COLUMN(V3)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="14"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1701,13 +2329,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>C1:C13 C22:C23 C25:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{456F7F48-20F7-4E73-8A50-6134AAE9277C}">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:R1048576</xm:sqref>
+          <xm:sqref>D2:Q13 D22:Q23 D25:Q1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1720,7 +2348,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1732,64 +2360,64 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>37</v>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
-        <v>38</v>
+      <c r="B10" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
comments added to scheduler
</commit_message>
<xml_diff>
--- a/Provider_Template.xlsx
+++ b/Provider_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminrutherford/PycharmProjects/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48681E6A-D328-9C49-B5E5-3393A7CA801F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006498CF-5330-6C47-8439-07A39A45236B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="64">
   <si>
     <t>Last</t>
   </si>
@@ -217,6 +217,30 @@
   </si>
   <si>
     <t>Marsha</t>
+  </si>
+  <si>
+    <t># 1 Crownpoint Healthcare Facility (CHCF)</t>
+  </si>
+  <si>
+    <t># 2 Thoreau Health Station (THS)</t>
+  </si>
+  <si>
+    <t># 3 Pueblo Pintado Health Center (PPHC)</t>
+  </si>
+  <si>
+    <t># 4 No Preference (NP)</t>
+  </si>
+  <si>
+    <t># 5 Administrative Time (Adm)</t>
+  </si>
+  <si>
+    <t># 6 Approved Leave (AL)</t>
+  </si>
+  <si>
+    <t># 7 Continuing Medical Education (CME)</t>
+  </si>
+  <si>
+    <t># 8 General Staff Meeting (GME)</t>
   </si>
 </sst>
 </file>
@@ -527,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1282,17 +1306,55 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Provider preferences column headers
</commit_message>
<xml_diff>
--- a/Provider_Template.xlsx
+++ b/Provider_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Google Drive\UNM\2021_spring\ECE435\project\DD_Branch\ece435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F835F06-1690-44B5-86C5-BACA519452B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CCA8C0-34C8-450A-806D-BF480FB41AD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="48">
   <si>
     <t>Last</t>
   </si>
@@ -58,68 +58,12 @@
     <t>Specialty</t>
   </si>
   <si>
-    <t>MON 
-PM</t>
-  </si>
-  <si>
-    <t>TUE 
-AM</t>
-  </si>
-  <si>
-    <t>TUE 
-PM</t>
-  </si>
-  <si>
-    <t>WED
-AM</t>
-  </si>
-  <si>
-    <t>WED
-PM</t>
-  </si>
-  <si>
-    <t>THU
-AM</t>
-  </si>
-  <si>
-    <t>THU
-PM</t>
-  </si>
-  <si>
-    <t>FRI
-AM</t>
-  </si>
-  <si>
-    <t>FRI
-PM</t>
-  </si>
-  <si>
-    <t>SAT
-AM</t>
-  </si>
-  <si>
-    <t>SAT
-PM</t>
-  </si>
-  <si>
-    <t>SUN
-AM</t>
-  </si>
-  <si>
-    <t>SUN
-PM</t>
-  </si>
-  <si>
     <t>Hour Limit</t>
   </si>
   <si>
     <t>Jane</t>
   </si>
   <si>
-    <t>MON
-AM</t>
-  </si>
-  <si>
     <t>CHCF</t>
   </si>
   <si>
@@ -226,6 +170,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PM</t>
   </si>
 </sst>
 </file>
@@ -253,40 +206,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -301,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -309,26 +243,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,242 +471,415 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S999"/>
+  <dimension ref="A1:AG999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="93" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.625" style="12" customWidth="1"/>
-    <col min="2" max="3" width="10.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="7.5" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="7.625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="7" style="3" customWidth="1"/>
-    <col min="19" max="26" width="7.625" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="3"/>
+    <col min="1" max="1" width="9.625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="18" width="7.875" style="3" customWidth="1"/>
+    <col min="19" max="29" width="8.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.875" style="3" customWidth="1"/>
+    <col min="31" max="33" width="8.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="40" width="7.625" style="3" customWidth="1"/>
+    <col min="41" max="16384" width="12.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:33" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>56</v>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/03
+ AM</v>
+      </c>
+      <c r="F1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/03
+ PM</v>
+      </c>
+      <c r="G1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/04
+ AM</v>
+      </c>
+      <c r="H1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/04
+ PM</v>
+      </c>
+      <c r="I1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/05
+ AM</v>
+      </c>
+      <c r="J1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/05
+ PM</v>
+      </c>
+      <c r="K1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/06
+ AM</v>
+      </c>
+      <c r="L1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/06
+ PM</v>
+      </c>
+      <c r="M1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/07
+ AM</v>
+      </c>
+      <c r="N1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/07
+ PM</v>
+      </c>
+      <c r="O1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/08
+ AM</v>
+      </c>
+      <c r="P1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/08
+ PM</v>
+      </c>
+      <c r="Q1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/09
+ AM</v>
+      </c>
+      <c r="R1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/09
+ PM</v>
+      </c>
+      <c r="S1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/10
+ AM</v>
+      </c>
+      <c r="T1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/10
+ PM</v>
+      </c>
+      <c r="U1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/11
+ AM</v>
+      </c>
+      <c r="V1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/11
+ PM</v>
+      </c>
+      <c r="W1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/12
+ AM</v>
+      </c>
+      <c r="X1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/12
+ PM</v>
+      </c>
+      <c r="Y1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/13
+ AM</v>
+      </c>
+      <c r="Z1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/13
+ PM</v>
+      </c>
+      <c r="AA1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/14
+ AM</v>
+      </c>
+      <c r="AB1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/14
+ PM</v>
+      </c>
+      <c r="AC1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/15
+ AM</v>
+      </c>
+      <c r="AD1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/15
+ PM</v>
+      </c>
+      <c r="AE1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," AM")</f>
+        <v>05/16
+ AM</v>
+      </c>
+      <c r="AF1" s="11" t="str">
+        <f ca="1">CONCATENATE(TEXT((Sheet2!$C$2)+(INT((COLUMN()-1)/2)-2), "mm/dd"),CHAR(10)," PM")</f>
+        <v>05/16
+ PM</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="B4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>2</v>
@@ -789,10 +888,10 @@
         <v>2</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>2</v>
@@ -801,328 +900,580 @@
         <v>2</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG8" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5" s="3">
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG9" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S7" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S8" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S9" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>2</v>
@@ -1155,45 +1506,87 @@
         <v>2</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S10" s="3">
+        <v>16</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>58</v>
+    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>2</v>
@@ -1202,142 +1595,268 @@
         <v>2</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S11" s="3">
+        <v>16</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG11" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>57</v>
+    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S12" s="3">
+        <v>16</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG12" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>57</v>
+    <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S13" s="3">
+        <v>16</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG13" s="3">
         <v>40</v>
       </c>
     </row>
@@ -2330,13 +2849,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D13 D22:D23 D24:D1048576</xm:sqref>
+          <xm:sqref>D22:R1048576 D1:D13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{456F7F48-20F7-4E73-8A50-6134AAE9277C}">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E22:F23 E2:F13 E24:F1048576</xm:sqref>
+          <xm:sqref>S2:T13 S22:T1048576 E2:F13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2346,79 +2865,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="26" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <f ca="1">IF(WEEKDAY(TODAY(),3)=0,TODAY(),TODAY()+(7-WEEKDAY(TODAY(),3)))</f>
+        <v>44319</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>28</v>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>29</v>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>